<commit_message>
probability threshold tuning logic
</commit_message>
<xml_diff>
--- a/AUDIO/MusicClassification/experiment_results.xlsx
+++ b/AUDIO/MusicClassification/experiment_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10710" windowHeight="4410"/>
   </bookViews>
   <sheets>
     <sheet name="Model training" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
   <si>
     <t>Model</t>
   </si>
@@ -222,13 +222,43 @@
     <t>Pog_MusicClf_Train version 21</t>
   </si>
   <si>
-    <t>melspec_iter2_ver2_resnext_run1n2</t>
-  </si>
-  <si>
-    <t>CosineAnnealingWarmRestarts (T_0=15)</t>
-  </si>
-  <si>
     <t>Early stopping at epoch 24</t>
+  </si>
+  <si>
+    <t>Pog_MusicClf_MelSpec_Aug version1</t>
+  </si>
+  <si>
+    <t>Pog_MusicClf_Resnext, melspec_iter2_ver2_resnext_run1</t>
+  </si>
+  <si>
+    <t>Pog_MusicClf_Resnext, melspec_aug_resnext_run2_fold0</t>
+  </si>
+  <si>
+    <t>Pog_MusicClf_Train version 30</t>
+  </si>
+  <si>
+    <t>Best loss at epoch 19</t>
+  </si>
+  <si>
+    <t>CosineAnnealingWarmRestarts (T_0=10)</t>
+  </si>
+  <si>
+    <t>COLAB pog-musicclf-train.ipynb pin revision: RESNET50_VAL_LOSS_1.5116</t>
+  </si>
+  <si>
+    <t>Pog_MusicClf_Resnext, melspec_aug_resnet_run1_fold0</t>
+  </si>
+  <si>
+    <t>Best loss at epoch 19, early stopping at epoch 30</t>
+  </si>
+  <si>
+    <t>Pog_MusicClf_Train version 33</t>
+  </si>
+  <si>
+    <t>Pog_MusicClf_Resnext, melspec_aug_effnet_run3</t>
+  </si>
+  <si>
+    <t>Best loss at epoch 9, early stopping at epoch 21</t>
   </si>
 </sst>
 </file>
@@ -613,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -623,7 +653,7 @@
     <col min="3" max="3" width="10.08984375" customWidth="1"/>
     <col min="4" max="4" width="7.81640625" customWidth="1"/>
     <col min="5" max="5" width="8.453125" customWidth="1"/>
-    <col min="9" max="9" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.36328125" customWidth="1"/>
     <col min="12" max="12" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.7265625" bestFit="1" customWidth="1"/>
@@ -1103,7 +1133,7 @@
         <v>21</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1">
@@ -1122,7 +1152,7 @@
         <v>64</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>34</v>
@@ -1134,65 +1164,188 @@
         <v>22</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.51895999999999998</v>
+      </c>
+      <c r="D10" s="1">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1">
+        <v>25</v>
+      </c>
+      <c r="F10" s="1">
+        <v>10</v>
+      </c>
+      <c r="G10" s="6">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1.5015000000000001</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0.50360000000000005</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.51536000000000004</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1">
+        <v>30</v>
+      </c>
+      <c r="F11" s="1">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6">
+        <v>2.7539999999999999E-3</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1.5306999999999999</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0.51139999999999997</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="T11" s="7" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.51417000000000002</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>40</v>
+      </c>
+      <c r="F12" s="1">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6">
+        <v>8.3169999999999997E-3</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1.5116000000000001</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.50460000000000005</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="T12" s="7" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>